<commit_message>
changes in Expenses incorporated
</commit_message>
<xml_diff>
--- a/reimbursement/src/main/resources/Config.xlsx
+++ b/reimbursement/src/main/resources/Config.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">chrome</t>
   </si>
   <si>
-    <t xml:space="preserve">automation</t>
+    <t xml:space="preserve">wild11</t>
   </si>
   <si>
     <t xml:space="preserve">DEBUG</t>
@@ -190,10 +190,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.12"/>

</xml_diff>

<commit_message>
Changes in Reimb classes
</commit_message>
<xml_diff>
--- a/reimbursement/src/main/resources/Config.xlsx
+++ b/reimbursement/src/main/resources/Config.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">chrome</t>
   </si>
   <si>
-    <t xml:space="preserve">wild11</t>
+    <t xml:space="preserve">wild1</t>
   </si>
   <si>
     <t xml:space="preserve">DEBUG</t>
@@ -193,7 +193,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.12"/>

</xml_diff>

<commit_message>
changes in reimb Form & expenses
</commit_message>
<xml_diff>
--- a/reimbursement/src/main/resources/Config.xlsx
+++ b/reimbursement/src/main/resources/Config.xlsx
@@ -46,10 +46,10 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">chrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wild1</t>
+    <t xml:space="preserve">firefox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automation</t>
   </si>
   <si>
     <t xml:space="preserve">DEBUG</t>
@@ -190,10 +190,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.12"/>

</xml_diff>